<commit_message>
feat: Weapon 데이터 추가
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/Enum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A0C8CD-1897-473B-B7EF-3633D3EB372D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BD0679-B45E-4D9A-88C5-47E56312433B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{F0B6D958-7859-4CF7-B5FD-305E8714B539}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>MonsterType</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,32 @@
   </si>
   <si>
     <t>Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EWeaponType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pistol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rifle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shotgun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sniper</t>
+  </si>
+  <si>
+    <t>Machinegun</t>
+  </si>
+  <si>
+    <t>Launcher</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,19 +449,24 @@
   <sheetPr codeName="Sheet8">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="7.875" customWidth="1"/>
+    <col min="3" max="3" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -461,6 +492,29 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>